<commit_message>
Work in progress - XML data source
</commit_message>
<xml_diff>
--- a/testdata/nodb/TestSheet.xlsx
+++ b/testdata/nodb/TestSheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E1C270-7424-4392-825D-DD3465F8BF1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07902B0F-2EAB-4BEB-8EFB-37FFE2F8AC04}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,37 +13,47 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Nadpis</t>
   </si>
   <si>
-    <t>Row 1</t>
-  </si>
-  <si>
-    <t>Row 2</t>
-  </si>
-  <si>
-    <t>Row 3</t>
-  </si>
-  <si>
-    <t>x</t>
+    <t>Entity2</t>
+  </si>
+  <si>
+    <t>Entity1</t>
+  </si>
+  <si>
+    <t>Entity3</t>
+  </si>
+  <si>
+    <t>Attr1</t>
+  </si>
+  <si>
+    <t>Attr2</t>
+  </si>
+  <si>
+    <t>Attr3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +74,15 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -96,11 +115,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -384,28 +404,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -416,41 +436,76 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2">
-        <f>$B$4</f>
-        <v>2</v>
-      </c>
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2">
         <f>$B$5</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="3">
-        <f>SUM(C3:C5)</f>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
+        <f>$B$9</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="str">
-        <f>'V100'!A1</f>
-        <v>x</v>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="3">
+        <f>SUM(C3:C9)</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -469,13 +524,7 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Work in progress - XML data source - mostly works, but ignores required data types
</commit_message>
<xml_diff>
--- a/testdata/nodb/TestSheet.xlsx
+++ b/testdata/nodb/TestSheet.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07902B0F-2EAB-4BEB-8EFB-37FFE2F8AC04}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F243C7C-EE27-4CC7-AA67-3C36AC8D6385}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="V100" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,6 +19,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>Nadpis</t>
   </si>
@@ -404,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,70 +443,82 @@
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2">
-        <f>$B$5</f>
-        <v>2</v>
-      </c>
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2"/>
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <f>$B$7</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2">
-        <f>$B$9</f>
-        <v>3</v>
-      </c>
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2"/>
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2">
+        <f>$B$11</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="3">
-        <f>SUM(C3:C9)</f>
-        <v>6</v>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="3">
+        <f>SUM(C3:C11)</f>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work in progress - better handling of preference for data type in data source
</commit_message>
<xml_diff>
--- a/testdata/nodb/TestSheet.xlsx
+++ b/testdata/nodb/TestSheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F243C7C-EE27-4CC7-AA67-3C36AC8D6385}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F536D398-45EF-4BE8-9C06-9E38B2A65336}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,7 +116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -125,6 +125,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,26 +406,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="5.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -436,25 +438,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="6">
+        <v>42016.51458333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="6">
+        <v>42016.51458333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="6">
+        <v>42016.51458333333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -466,25 +477,34 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="6">
+        <v>42016.51458333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="6">
+        <v>42016.51458333333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="6">
+        <v>42016.51458333333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -496,24 +516,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="6">
+        <v>42016.51458333333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="6">
+        <v>42016.51458333333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="6">
+        <v>42016.51458333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="3">

</xml_diff>